<commit_message>
add os, port, vuln report; almost finished
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -50,8 +50,9 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -134,91 +135,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>